<commit_message>
Normalizando quebras de linha
</commit_message>
<xml_diff>
--- a/Documentação/BackLog.xlsx
+++ b/Documentação/BackLog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/429a2cd294968864/Documentos/ProximoPasso/ProximoPasso/Documentação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/429a2cd294968864/Área de Trabalho/Proximopasso/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{535C6DBB-ADAD-4530-987A-D8E71E255342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0311551-E26F-4CD5-9D04-5449CA7C4E66}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{535C6DBB-ADAD-4530-987A-D8E71E255342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B623AC7-7B34-4456-A997-A59C440302E0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>PROJETO BACKLOG</t>
   </si>
@@ -180,18 +180,6 @@
   </si>
   <si>
     <t>3-Semana</t>
-  </si>
-  <si>
-    <t>Soma</t>
-  </si>
-  <si>
-    <t>Média</t>
-  </si>
-  <si>
-    <t>Soma Acumulada</t>
-  </si>
-  <si>
-    <t>Contagem</t>
   </si>
 </sst>
 </file>
@@ -528,10 +516,56 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
         <right style="medium">
           <color indexed="64"/>
         </right>
@@ -545,8 +579,12 @@
         <right style="medium">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -579,25 +617,19 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right/>
-        <top/>
-        <bottom/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -625,74 +657,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
@@ -705,6 +669,30 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1008,7 +996,10 @@
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47</c:v>
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1076,7 +1067,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1930,12 +1924,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F158064E-290A-4CC0-B584-891006F4F0BB}" name="Tabela2" displayName="Tabela2" ref="C3:H17" totalsRowShown="0" tableBorderDxfId="12">
   <autoFilter ref="C3:H17" xr:uid="{F158064E-290A-4CC0-B584-891006F4F0BB}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C73CE283-21D6-4B9F-95B6-46577DCC78CE}" name="Requisito" dataDxfId="11" totalsRowDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{4B60BF41-E3D5-4BBA-9A71-0A47B3D33D85}" name="Descrição" dataDxfId="10" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{927EEA8A-278F-4381-A742-AE735F259419}" name="Classificação" dataDxfId="9" totalsRowDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{9A9344F6-5C90-4DC0-882B-3ACCFA815007}" name="Tamanho" dataDxfId="8" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{7F98729B-10DC-4DDC-976D-9CB83B9B6D16}" name="Tam(Fibonacci)" dataDxfId="7" totalsRowDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{D99A6B89-10B3-419A-8F09-33FC36095ABA}" name="Prioridade" dataDxfId="6" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C73CE283-21D6-4B9F-95B6-46577DCC78CE}" name="Requisito" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{4B60BF41-E3D5-4BBA-9A71-0A47B3D33D85}" name="Descrição" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{927EEA8A-278F-4381-A742-AE735F259419}" name="Classificação" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{9A9344F6-5C90-4DC0-882B-3ACCFA815007}" name="Tamanho" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{7F98729B-10DC-4DDC-976D-9CB83B9B6D16}" name="Tam(Fibonacci)" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D99A6B89-10B3-419A-8F09-33FC36095ABA}" name="Prioridade" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2260,8 +2254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2403,10 +2397,10 @@
         <v>48</v>
       </c>
       <c r="N5" s="38">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O5" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2436,6 +2430,12 @@
       </c>
       <c r="M6">
         <v>50</v>
+      </c>
+      <c r="N6">
+        <v>50</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2689,23 +2689,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A729CFA7192B0F4AA60BE2DF65F4BC74" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a10fb9a05e03931258d7cbef6b140aea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52deff43771b9580cfe5b392a2218df8" ns3:_="">
     <xsd:import namespace="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
@@ -2855,10 +2838,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4F8EAC-B7AA-48FA-A973-158E61613278}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17B39212-3AF5-40FE-813D-54F0FAA5F059}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2880,19 +2890,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17B39212-3AF5-40FE-813D-54F0FAA5F059}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4F8EAC-B7AA-48FA-A973-158E61613278}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>